<commit_message>
push to main 05.08.25
</commit_message>
<xml_diff>
--- a/public/sample/weight_variation_sample.xlsx
+++ b/public/sample/weight_variation_sample.xlsx
@@ -31,7 +31,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>product_no</t>
+    <t>material_code</t>
   </si>
   <si>
     <t>weight</t>
@@ -1019,15 +1019,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="7.14285714285714" customWidth="1"/>
-    <col min="3" max="3" width="13.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="5.42857142857143" customWidth="1"/>
+    <col min="1" max="1" width="14.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="7.71428571428571" customWidth="1"/>
+    <col min="3" max="3" width="14.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="11.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>